<commit_message>
Update footer and document summary
</commit_message>
<xml_diff>
--- a/Excel/TC001_Login.xlsx
+++ b/Excel/TC001_Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Selenium_2024\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07285B6E-EC66-4C4B-AE85-A69AF0266302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8DDC9A-7580-4CD7-8002-26B951BC4DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F15E9A0-1C50-4655-9A11-8F4BEDD34A56}"/>
+    <workbookView xWindow="8850" yWindow="330" windowWidth="12210" windowHeight="15150" xr2:uid="{2F15E9A0-1C50-4655-9A11-8F4BEDD34A56}"/>
   </bookViews>
   <sheets>
     <sheet name="TC001" sheetId="1" r:id="rId1"/>
@@ -459,6 +459,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -473,9 +476,6 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>

</xml_diff>